<commit_message>
add case history tab component to ES
</commit_message>
<xml_diff>
--- a/aat/src/resource/CCD_CNP_27.xlsx
+++ b/aat/src/resource/CCD_CNP_27.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A533913\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/code/ccd/ccd-definition-store-api/aat/src/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{427A6C7C-B7FE-4CBA-907E-7C6E6F05AF53}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994F7540-D464-3047-B730-B47B7DA7E545}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2256" windowWidth="28800" windowHeight="15936" tabRatio="823" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1080" windowWidth="28800" windowHeight="15940" tabRatio="823" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1855" uniqueCount="275">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -862,6 +862,24 @@
   </si>
   <si>
     <t>Radio Value 2</t>
+  </si>
+  <si>
+    <t>HistoryComponentField</t>
+  </si>
+  <si>
+    <t>A `HistoryComponent` field</t>
+  </si>
+  <si>
+    <t>History tab component</t>
+  </si>
+  <si>
+    <t>CaseHistoryViewer</t>
+  </si>
+  <si>
+    <t>HistoryTab</t>
+  </si>
+  <si>
+    <t>History Tab</t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1096,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1101,6 +1119,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -1186,7 +1210,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1292,6 +1316,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="4" applyAlignment="1"/>
     <xf numFmtId="49" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1627,16 +1652,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" customWidth="1"/>
-    <col min="5" max="5" width="43.77734375" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="43.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1651,7 +1676,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -1664,7 +1689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -1681,7 +1706,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>42736</v>
       </c>
@@ -1723,17 +1748,17 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -1749,7 +1774,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" s="30" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="30" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -1765,7 +1790,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -1785,7 +1810,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
         <v>42736</v>
       </c>
@@ -1803,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="23">
         <v>42736</v>
       </c>
@@ -1821,7 +1846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23">
         <v>42736</v>
       </c>
@@ -1839,7 +1864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="23">
         <v>42736</v>
       </c>
@@ -1876,7 +1901,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0900-000004000000}">
           <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$34</xm:f>
+            <xm:f>CaseField!$D$4:$D$35</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D7</xm:sqref>
         </x14:dataValidation>
@@ -1897,18 +1922,18 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" style="70" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="71" customWidth="1"/>
-    <col min="3" max="3" width="29.77734375" style="71" customWidth="1"/>
-    <col min="4" max="4" width="19.77734375" style="71" customWidth="1"/>
-    <col min="5" max="5" width="20.21875" style="71" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" style="70" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="71" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" style="71" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" style="71" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="71" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" style="71" customWidth="1"/>
-    <col min="7" max="16384" width="8.77734375" style="14"/>
+    <col min="7" max="16384" width="8.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="62" t="s">
         <v>130</v>
       </c>
@@ -1924,7 +1949,7 @@
       <c r="E1" s="66"/>
       <c r="F1" s="66"/>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="48" x14ac:dyDescent="0.15">
       <c r="A2" s="67"/>
       <c r="B2" s="67"/>
       <c r="C2" s="68" t="s">
@@ -1940,7 +1965,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="69" t="s">
         <v>8</v>
       </c>
@@ -1960,7 +1985,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>42736</v>
       </c>
@@ -1978,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -2015,7 +2040,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{00000000-0002-0000-0A00-000003000000}">
           <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$34</xm:f>
+            <xm:f>CaseField!$D$4:$D$35</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D5</xm:sqref>
         </x14:dataValidation>
@@ -2036,7 +2061,7 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -2046,7 +2071,7 @@
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -2062,7 +2087,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" s="30" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="30" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
       <c r="C2" s="31" t="s">
@@ -2078,7 +2103,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -2098,7 +2123,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
         <v>42736</v>
       </c>
@@ -2116,7 +2141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="23">
         <v>42736</v>
       </c>
@@ -2134,7 +2159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23">
         <v>42736</v>
       </c>
@@ -2152,7 +2177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="23">
         <v>42736</v>
       </c>
@@ -2189,7 +2214,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0B00-000004000000}">
           <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$34</xm:f>
+            <xm:f>CaseField!$D$4:$D$35</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D7</xm:sqref>
         </x14:dataValidation>
@@ -2204,25 +2229,25 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" customWidth="1"/>
     <col min="4" max="4" width="31.6640625" customWidth="1"/>
     <col min="5" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="16.33203125" customWidth="1"/>
-    <col min="8" max="8" width="40.77734375" customWidth="1"/>
+    <col min="8" max="8" width="40.83203125" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -2241,7 +2266,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
       <c r="C2" s="31" t="s">
@@ -2266,7 +2291,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -2295,7 +2320,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25">
         <v>42736</v>
       </c>
@@ -2322,7 +2347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27">
         <v>42736</v>
       </c>
@@ -2349,7 +2374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27">
         <v>42736</v>
       </c>
@@ -2376,7 +2401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27">
         <v>42736</v>
       </c>
@@ -2403,7 +2428,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27">
         <v>42736</v>
       </c>
@@ -2430,7 +2455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27">
         <v>42736</v>
       </c>
@@ -2457,7 +2482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27">
         <v>42736</v>
       </c>
@@ -2484,7 +2509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27">
         <v>42736</v>
       </c>
@@ -2511,7 +2536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27">
         <v>42736</v>
       </c>
@@ -2538,7 +2563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27">
         <v>42736</v>
       </c>
@@ -2565,7 +2590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="27">
         <v>42736</v>
       </c>
@@ -2592,7 +2617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="27">
         <v>42736</v>
       </c>
@@ -2619,7 +2644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27">
         <v>42736</v>
       </c>
@@ -2646,7 +2671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27">
         <v>42736</v>
       </c>
@@ -2673,7 +2698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="27">
         <v>42736</v>
       </c>
@@ -2700,7 +2725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="27">
         <v>42736</v>
       </c>
@@ -2727,34 +2752,34 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="27">
         <v>42736</v>
       </c>
       <c r="B20" s="27"/>
       <c r="C20" s="14" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="D20" s="28" t="s">
         <v>56</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>211</v>
+        <v>273</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>212</v>
+        <v>274</v>
       </c>
       <c r="G20" s="28">
-        <v>1</v>
-      </c>
-      <c r="H20" s="28" t="s">
-        <v>135</v>
+        <v>4</v>
+      </c>
+      <c r="H20" s="42" t="s">
+        <v>269</v>
       </c>
       <c r="I20" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="27">
         <v>42736</v>
       </c>
@@ -2775,13 +2800,13 @@
         <v>1</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I21" s="28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="27">
         <v>42736</v>
       </c>
@@ -2802,13 +2827,13 @@
         <v>1</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I22" s="28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="27">
         <v>42736</v>
       </c>
@@ -2828,14 +2853,14 @@
       <c r="G23" s="28">
         <v>1</v>
       </c>
-      <c r="H23" s="42" t="s">
-        <v>144</v>
+      <c r="H23" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="I23" s="28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27">
         <v>42736</v>
       </c>
@@ -2856,13 +2881,13 @@
         <v>1</v>
       </c>
       <c r="H24" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I24" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="27">
         <v>42736</v>
       </c>
@@ -2874,22 +2899,22 @@
         <v>56</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G25" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H25" s="42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I25" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27">
         <v>42736</v>
       </c>
@@ -2910,13 +2935,13 @@
         <v>2</v>
       </c>
       <c r="H26" s="42" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="I26" s="28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="27">
         <v>42736</v>
       </c>
@@ -2937,13 +2962,13 @@
         <v>2</v>
       </c>
       <c r="H27" s="42" t="s">
-        <v>247</v>
+        <v>158</v>
       </c>
       <c r="I27" s="28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="27">
         <v>42736</v>
       </c>
@@ -2964,13 +2989,13 @@
         <v>2</v>
       </c>
       <c r="H28" s="42" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="I28" s="28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="27">
         <v>42736</v>
       </c>
@@ -2991,13 +3016,13 @@
         <v>2</v>
       </c>
       <c r="H29" s="42" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I29" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="27">
         <v>42736</v>
       </c>
@@ -3018,13 +3043,13 @@
         <v>2</v>
       </c>
       <c r="H30" s="42" t="s">
-        <v>258</v>
+        <v>160</v>
       </c>
       <c r="I30" s="28">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="27">
         <v>42736</v>
       </c>
@@ -3045,13 +3070,13 @@
         <v>2</v>
       </c>
       <c r="H31" s="42" t="s">
-        <v>170</v>
+        <v>258</v>
       </c>
       <c r="I31" s="28">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="27">
         <v>42736</v>
       </c>
@@ -3063,22 +3088,22 @@
         <v>56</v>
       </c>
       <c r="E32" s="42" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="G32" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H32" s="42" t="s">
-        <v>225</v>
+        <v>170</v>
       </c>
       <c r="I32" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="27">
         <v>42736</v>
       </c>
@@ -3099,13 +3124,13 @@
         <v>3</v>
       </c>
       <c r="H33" s="42" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="I33" s="28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="27">
         <v>42736</v>
       </c>
@@ -3126,21 +3151,75 @@
         <v>3</v>
       </c>
       <c r="H34" s="42" t="s">
+        <v>240</v>
+      </c>
+      <c r="I34" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="27">
+        <v>42736</v>
+      </c>
+      <c r="B35" s="27"/>
+      <c r="C35" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="G35" s="28">
+        <v>3</v>
+      </c>
+      <c r="H35" s="42" t="s">
         <v>243</v>
       </c>
-      <c r="I34" s="28">
+      <c r="I35" s="28">
         <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="27">
+        <v>42736</v>
+      </c>
+      <c r="B36" s="27"/>
+      <c r="C36" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>274</v>
+      </c>
+      <c r="G36" s="28">
+        <v>4</v>
+      </c>
+      <c r="H36" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="I36" s="28">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="I4:I34 G4:G34" xr:uid="{00000000-0002-0000-0C00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G36 I4:I36" xr:uid="{00000000-0002-0000-0C00-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A34" xr:uid="{00000000-0002-0000-0C00-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A36" xr:uid="{00000000-0002-0000-0C00-000002000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B34" xr:uid="{00000000-0002-0000-0C00-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B36" xr:uid="{00000000-0002-0000-0C00-000000000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -3162,17 +3241,17 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="28.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
@@ -3187,7 +3266,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="3" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="37" t="s">
         <v>8</v>
       </c>
@@ -3207,7 +3286,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="72">
         <v>42736</v>
       </c>
@@ -3246,15 +3325,15 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -3269,7 +3348,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" s="30" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="30" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
       <c r="C2" s="31" t="s">
@@ -3282,7 +3361,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -3299,7 +3378,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="29">
         <v>42736</v>
       </c>
@@ -3314,7 +3393,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="14" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="29">
         <v>42736</v>
       </c>
@@ -3348,18 +3427,18 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.21875" style="61" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="61" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="61" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" style="61" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="61" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="61" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" style="61" customWidth="1"/>
     <col min="5" max="5" width="27" style="61" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" style="61" customWidth="1"/>
-    <col min="7" max="16384" width="8.77734375" style="54"/>
+    <col min="6" max="6" width="14.5" style="61" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="49" t="s">
         <v>128</v>
       </c>
@@ -3375,7 +3454,7 @@
       <c r="E1" s="53"/>
       <c r="F1" s="53"/>
     </row>
-    <row r="2" spans="1:6" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="55"/>
       <c r="B2" s="55"/>
       <c r="C2" s="56" t="s">
@@ -3391,7 +3470,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="57" t="s">
         <v>8</v>
       </c>
@@ -3411,7 +3490,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="59">
         <v>42736</v>
       </c>
@@ -3429,7 +3508,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="59">
         <v>42736</v>
       </c>
@@ -3447,7 +3526,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="59">
         <v>42736</v>
       </c>
@@ -3465,7 +3544,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="59">
         <v>42736</v>
       </c>
@@ -3483,7 +3562,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="59">
         <v>42736</v>
       </c>
@@ -3501,7 +3580,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="59">
         <v>42736</v>
       </c>
@@ -3538,16 +3617,16 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.77734375" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
@@ -3563,7 +3642,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" s="30" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="30" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -3579,7 +3658,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="33" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -3599,7 +3678,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="72">
         <v>42736</v>
       </c>
@@ -3616,7 +3695,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="72">
         <v>42736</v>
       </c>
@@ -3633,7 +3712,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="72">
         <v>42736</v>
       </c>
@@ -3650,7 +3729,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="72">
         <v>42736</v>
       </c>
@@ -3667,7 +3746,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="72">
         <v>42736</v>
       </c>
@@ -3684,7 +3763,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="72">
         <v>42736</v>
       </c>
@@ -3701,7 +3780,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="72">
         <v>42736</v>
       </c>
@@ -3718,7 +3797,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="72">
         <v>42736</v>
       </c>
@@ -3735,7 +3814,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="72">
         <v>42736</v>
       </c>
@@ -3752,7 +3831,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="72">
         <v>42736</v>
       </c>
@@ -3769,7 +3848,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="72">
         <v>42736</v>
       </c>
@@ -3786,7 +3865,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="72">
         <v>42736</v>
       </c>
@@ -3816,22 +3895,22 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
@@ -3846,7 +3925,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -3862,7 +3941,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="33" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -3882,7 +3961,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="72">
         <v>42736</v>
       </c>
@@ -3899,7 +3978,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="72">
         <v>42736</v>
       </c>
@@ -3916,7 +3995,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="72">
         <v>42736</v>
       </c>
@@ -3933,7 +4012,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="72">
         <v>42736</v>
       </c>
@@ -3950,7 +4029,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="72">
         <v>42736</v>
       </c>
@@ -3967,7 +4046,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="72">
         <v>42736</v>
       </c>
@@ -3984,7 +4063,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="72">
         <v>42736</v>
       </c>
@@ -4001,7 +4080,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="72">
         <v>42736</v>
       </c>
@@ -4018,7 +4097,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="72">
         <v>42736</v>
       </c>
@@ -4035,7 +4114,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="72">
         <v>42736</v>
       </c>
@@ -4052,7 +4131,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="72">
         <v>42736</v>
       </c>
@@ -4069,7 +4148,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="72">
         <v>42736</v>
       </c>
@@ -4086,7 +4165,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="72">
         <v>42736</v>
       </c>
@@ -4104,7 +4183,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="72">
         <v>42736</v>
       </c>
@@ -4121,7 +4200,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="72">
         <v>42736</v>
       </c>
@@ -4139,7 +4218,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="72">
         <v>42736</v>
       </c>
@@ -4156,15 +4235,15 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="72">
         <v>42736</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>135</v>
+        <v>234</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>269</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>236</v>
@@ -4173,7 +4252,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="72">
         <v>42736</v>
       </c>
@@ -4181,7 +4260,7 @@
         <v>251</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>236</v>
@@ -4190,7 +4269,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="72">
         <v>42736</v>
       </c>
@@ -4198,7 +4277,7 @@
         <v>251</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>236</v>
@@ -4207,15 +4286,15 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="72">
         <v>42736</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="D23" s="42" t="s">
-        <v>144</v>
+      <c r="D23" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>236</v>
@@ -4224,7 +4303,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="72">
         <v>42736</v>
       </c>
@@ -4232,7 +4311,7 @@
         <v>251</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>236</v>
@@ -4241,7 +4320,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="72">
         <v>42736</v>
       </c>
@@ -4249,7 +4328,7 @@
         <v>251</v>
       </c>
       <c r="D25" s="42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E25" s="14" t="s">
         <v>236</v>
@@ -4258,7 +4337,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="72">
         <v>42736</v>
       </c>
@@ -4266,7 +4345,7 @@
         <v>251</v>
       </c>
       <c r="D26" s="42" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>236</v>
@@ -4275,7 +4354,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="72">
         <v>42736</v>
       </c>
@@ -4283,7 +4362,7 @@
         <v>251</v>
       </c>
       <c r="D27" s="42" t="s">
-        <v>247</v>
+        <v>158</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>236</v>
@@ -4292,7 +4371,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="72">
         <v>42736</v>
       </c>
@@ -4300,7 +4379,7 @@
         <v>251</v>
       </c>
       <c r="D28" s="42" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>236</v>
@@ -4309,7 +4388,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="72">
         <v>42736</v>
       </c>
@@ -4317,7 +4396,7 @@
         <v>251</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>236</v>
@@ -4326,7 +4405,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="72">
         <v>42736</v>
       </c>
@@ -4334,7 +4413,7 @@
         <v>251</v>
       </c>
       <c r="D30" s="42" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>236</v>
@@ -4343,15 +4422,15 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="72">
         <v>42736</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="D31" s="24" t="s">
-        <v>243</v>
+      <c r="D31" s="42" t="s">
+        <v>170</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>236</v>
@@ -4360,15 +4439,15 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="72">
         <v>42736</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="D32" s="42" t="s">
-        <v>240</v>
+      <c r="D32" s="24" t="s">
+        <v>243</v>
       </c>
       <c r="E32" s="14" t="s">
         <v>236</v>
@@ -4377,7 +4456,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="72">
         <v>42736</v>
       </c>
@@ -4385,7 +4464,7 @@
         <v>251</v>
       </c>
       <c r="D33" s="42" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="E33" s="14" t="s">
         <v>236</v>
@@ -4394,7 +4473,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="72">
         <v>42736</v>
       </c>
@@ -4402,12 +4481,46 @@
         <v>251</v>
       </c>
       <c r="D34" s="42" t="s">
-        <v>258</v>
+        <v>225</v>
       </c>
       <c r="E34" s="14" t="s">
         <v>236</v>
       </c>
       <c r="F34" s="24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="72">
+        <v>42736</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="72">
+        <v>42736</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="F36" s="24" t="s">
         <v>124</v>
       </c>
     </row>
@@ -4430,20 +4543,20 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.77734375" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -4462,7 +4575,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" s="30" customFormat="1" ht="73.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="30" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -4487,7 +4600,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -4516,7 +4629,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="11">
         <v>42736</v>
       </c>
@@ -4537,7 +4650,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -4579,28 +4692,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.77734375" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" customWidth="1"/>
     <col min="4" max="4" width="41.33203125" customWidth="1"/>
-    <col min="5" max="5" width="40.77734375" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" customWidth="1"/>
+    <col min="5" max="5" width="40.83203125" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
     <col min="7" max="8" width="37" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="10" max="10" width="20.33203125" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="13" width="8.77734375" customWidth="1"/>
+    <col min="12" max="13" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4620,7 +4733,7 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:13" s="30" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="30" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -4653,7 +4766,7 @@
       <c r="L2" s="32"/>
       <c r="M2" s="32"/>
     </row>
-    <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -4694,7 +4807,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>42736</v>
       </c>
@@ -4723,7 +4836,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -4752,7 +4865,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>42736</v>
       </c>
@@ -4781,7 +4894,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -4810,7 +4923,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -4839,7 +4952,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="13">
         <v>42736</v>
       </c>
@@ -4868,7 +4981,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="13">
         <v>42736</v>
       </c>
@@ -4897,7 +5010,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13">
         <v>42736</v>
       </c>
@@ -4926,7 +5039,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13">
         <v>42736</v>
       </c>
@@ -4955,7 +5068,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13">
         <v>42736</v>
       </c>
@@ -4986,7 +5099,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13">
         <v>42736</v>
       </c>
@@ -5017,7 +5130,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13">
         <v>42736</v>
       </c>
@@ -5048,7 +5161,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13">
         <v>42736</v>
       </c>
@@ -5077,7 +5190,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13">
         <v>42736</v>
       </c>
@@ -5106,7 +5219,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13">
         <v>42736</v>
       </c>
@@ -5135,7 +5248,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="13">
         <v>42736</v>
       </c>
@@ -5166,27 +5279,27 @@
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13">
         <v>42736</v>
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="F20" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="G20" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="H20" s="28"/>
+        <v>234</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="F20" s="42" t="s">
+        <v>271</v>
+      </c>
+      <c r="G20" s="75" t="s">
+        <v>272</v>
+      </c>
+      <c r="H20" s="42"/>
       <c r="I20" s="28" t="s">
         <v>26</v>
       </c>
@@ -5195,7 +5308,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="13">
         <v>42736</v>
       </c>
@@ -5204,16 +5317,16 @@
         <v>251</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H21" s="28"/>
       <c r="I21" s="28" t="s">
@@ -5224,7 +5337,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="13">
         <v>42736</v>
       </c>
@@ -5233,16 +5346,16 @@
         <v>251</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="G22" s="42" t="s">
-        <v>30</v>
+        <v>142</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>28</v>
       </c>
       <c r="H22" s="28"/>
       <c r="I22" s="28" t="s">
@@ -5253,7 +5366,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="13">
         <v>42736</v>
       </c>
@@ -5261,17 +5374,17 @@
       <c r="C23" s="28" t="s">
         <v>251</v>
       </c>
-      <c r="D23" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="E23" s="42" t="s">
-        <v>145</v>
-      </c>
-      <c r="F23" s="42" t="s">
-        <v>148</v>
+      <c r="D23" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>141</v>
       </c>
       <c r="G23" s="42" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="H23" s="28"/>
       <c r="I23" s="28" t="s">
@@ -5282,7 +5395,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="13">
         <v>42736</v>
       </c>
@@ -5291,16 +5404,16 @@
         <v>251</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F24" s="42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G24" s="42" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="H24" s="28"/>
       <c r="I24" s="28" t="s">
@@ -5311,7 +5424,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="13">
         <v>42736</v>
       </c>
@@ -5320,16 +5433,16 @@
         <v>251</v>
       </c>
       <c r="D25" s="42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F25" s="42" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G25" s="42" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="H25" s="28"/>
       <c r="I25" s="28" t="s">
@@ -5340,7 +5453,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="13">
         <v>42736</v>
       </c>
@@ -5349,16 +5462,16 @@
         <v>251</v>
       </c>
       <c r="D26" s="42" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="E26" s="42" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F26" s="42" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G26" s="42" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="H26" s="28"/>
       <c r="I26" s="28" t="s">
@@ -5369,7 +5482,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="13">
         <v>42736</v>
       </c>
@@ -5378,16 +5491,16 @@
         <v>251</v>
       </c>
       <c r="D27" s="42" t="s">
-        <v>247</v>
+        <v>158</v>
       </c>
       <c r="E27" s="42" t="s">
-        <v>248</v>
+        <v>153</v>
       </c>
       <c r="F27" s="42" t="s">
-        <v>249</v>
+        <v>154</v>
       </c>
       <c r="G27" s="42" t="s">
-        <v>250</v>
+        <v>27</v>
       </c>
       <c r="H27" s="28"/>
       <c r="I27" s="28" t="s">
@@ -5398,7 +5511,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="13">
         <v>42736</v>
       </c>
@@ -5407,16 +5520,16 @@
         <v>251</v>
       </c>
       <c r="D28" s="42" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>157</v>
+        <v>248</v>
       </c>
       <c r="F28" s="42" t="s">
-        <v>159</v>
+        <v>249</v>
       </c>
       <c r="G28" s="42" t="s">
-        <v>155</v>
+        <v>250</v>
       </c>
       <c r="H28" s="28"/>
       <c r="I28" s="28" t="s">
@@ -5427,7 +5540,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="13">
         <v>42736</v>
       </c>
@@ -5436,20 +5549,18 @@
         <v>251</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F29" s="42" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G29" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="H29" s="42" t="s">
-        <v>163</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="H29" s="28"/>
       <c r="I29" s="28" t="s">
         <v>26</v>
       </c>
@@ -5458,7 +5569,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="13">
         <v>42736</v>
       </c>
@@ -5467,19 +5578,19 @@
         <v>251</v>
       </c>
       <c r="D30" s="42" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E30" s="42" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="F30" s="42" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G30" s="42" t="s">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="H30" s="42" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="I30" s="28" t="s">
         <v>26</v>
@@ -5489,7 +5600,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="13">
         <v>42736</v>
       </c>
@@ -5498,19 +5609,19 @@
         <v>251</v>
       </c>
       <c r="D31" s="42" t="s">
-        <v>240</v>
+        <v>170</v>
       </c>
       <c r="E31" s="42" t="s">
-        <v>241</v>
+        <v>171</v>
       </c>
       <c r="F31" s="42" t="s">
-        <v>242</v>
+        <v>172</v>
       </c>
       <c r="G31" s="42" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="H31" s="42" t="s">
-        <v>25</v>
+        <v>173</v>
       </c>
       <c r="I31" s="28" t="s">
         <v>26</v>
@@ -5520,7 +5631,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="13">
         <v>42736</v>
       </c>
@@ -5529,18 +5640,20 @@
         <v>251</v>
       </c>
       <c r="D32" s="42" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="E32" s="42" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
       <c r="F32" s="42" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="G32" s="42" t="s">
-        <v>228</v>
-      </c>
-      <c r="H32" s="42"/>
+        <v>80</v>
+      </c>
+      <c r="H32" s="42" t="s">
+        <v>25</v>
+      </c>
       <c r="I32" s="28" t="s">
         <v>26</v>
       </c>
@@ -5549,7 +5662,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="13">
         <v>42736</v>
       </c>
@@ -5558,16 +5671,16 @@
         <v>251</v>
       </c>
       <c r="D33" s="42" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="E33" s="42" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="F33" s="42" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="G33" s="42" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="H33" s="42"/>
       <c r="I33" s="28" t="s">
@@ -5578,7 +5691,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="13">
         <v>42736</v>
       </c>
@@ -5587,20 +5700,18 @@
         <v>251</v>
       </c>
       <c r="D34" s="42" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="E34" s="42" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="F34" s="42" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="G34" s="42" t="s">
-        <v>261</v>
-      </c>
-      <c r="H34" s="42" t="s">
-        <v>262</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="H34" s="42"/>
       <c r="I34" s="28" t="s">
         <v>26</v>
       </c>
@@ -5609,12 +5720,72 @@
         <v>117</v>
       </c>
     </row>
+    <row r="35" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="E35" s="42" t="s">
+        <v>259</v>
+      </c>
+      <c r="F35" s="42" t="s">
+        <v>260</v>
+      </c>
+      <c r="G35" s="42" t="s">
+        <v>261</v>
+      </c>
+      <c r="H35" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="I35" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B36" s="13"/>
+      <c r="C36" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="F36" s="42" t="s">
+        <v>271</v>
+      </c>
+      <c r="G36" s="75" t="s">
+        <v>272</v>
+      </c>
+      <c r="H36" s="42"/>
+      <c r="I36" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J36" s="28"/>
+      <c r="K36" s="28" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A34" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A36" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B34" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B36" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -5636,15 +5807,15 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="31.6640625" customWidth="1"/>
     <col min="5" max="5" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -5659,7 +5830,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -5672,7 +5843,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -5689,7 +5860,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="15">
         <v>42736</v>
       </c>
@@ -5704,7 +5875,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="15">
         <v>42736</v>
       </c>
@@ -5719,7 +5890,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="15">
         <v>42736</v>
       </c>
@@ -5734,7 +5905,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="15">
         <v>42736</v>
       </c>
@@ -5749,7 +5920,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="15">
         <v>42736</v>
       </c>
@@ -5764,7 +5935,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="15">
         <v>42736</v>
       </c>
@@ -5779,7 +5950,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="15">
         <v>42736</v>
       </c>
@@ -5794,7 +5965,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="15">
         <v>42736</v>
       </c>
@@ -5809,7 +5980,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="15">
         <v>42736</v>
       </c>
@@ -5824,7 +5995,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="15">
         <v>42736</v>
       </c>
@@ -5839,7 +6010,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="15">
         <v>42736</v>
       </c>
@@ -5880,7 +6051,7 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -5889,15 +6060,15 @@
     <col min="5" max="5" width="28.33203125" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="24.77734375" customWidth="1"/>
-    <col min="9" max="9" width="24.77734375" style="14" customWidth="1"/>
+    <col min="8" max="8" width="24.83203125" customWidth="1"/>
+    <col min="9" max="9" width="24.83203125" style="14" customWidth="1"/>
     <col min="10" max="10" width="37" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
-    <col min="13" max="14" width="8.77734375" customWidth="1"/>
+    <col min="13" max="14" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -5918,7 +6089,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -5954,7 +6125,7 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -5998,7 +6169,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>42736</v>
       </c>
@@ -6028,7 +6199,7 @@
       <c r="M4" s="35"/>
       <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -6060,7 +6231,7 @@
       <c r="M5" s="35"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="11">
         <v>42736</v>
       </c>
@@ -6088,7 +6259,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -6118,7 +6289,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -6172,18 +6343,18 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.33203125" customWidth="1"/>
     <col min="5" max="5" width="31.6640625" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -6200,7 +6371,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" ht="61.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="61" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -6213,7 +6384,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -6236,7 +6407,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="11">
         <v>42736</v>
       </c>
@@ -6255,7 +6426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -6274,7 +6445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>42736</v>
       </c>
@@ -6293,7 +6464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -6312,7 +6483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -6331,7 +6502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="13">
         <v>42736</v>
       </c>
@@ -6380,11 +6551,11 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.6640625" customWidth="1"/>
     <col min="6" max="6" width="45.33203125" customWidth="1"/>
@@ -6394,14 +6565,14 @@
     <col min="10" max="10" width="29.6640625" style="30" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="32" style="30" customWidth="1"/>
     <col min="12" max="12" width="31.33203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.77734375" style="30" customWidth="1"/>
+    <col min="13" max="13" width="29.83203125" style="30" customWidth="1"/>
     <col min="14" max="14" width="26.6640625" style="30" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="29.33203125" style="30" customWidth="1"/>
     <col min="16" max="16" width="23.6640625" customWidth="1"/>
-    <col min="17" max="17" width="31.21875" customWidth="1"/>
+    <col min="17" max="17" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -6420,7 +6591,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -6469,7 +6640,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -6522,7 +6693,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="11">
         <v>42736</v>
       </c>
@@ -6551,7 +6722,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -6588,7 +6759,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>42736</v>
       </c>
@@ -6625,7 +6796,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -6662,7 +6833,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -6699,7 +6870,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="13">
         <v>42736</v>
       </c>
@@ -6736,7 +6907,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="13">
         <v>42736</v>
       </c>
@@ -6771,7 +6942,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13">
         <v>42736</v>
       </c>
@@ -6808,7 +6979,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13">
         <v>42736</v>
       </c>
@@ -6845,7 +7016,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13">
         <v>42736</v>
       </c>
@@ -6882,7 +7053,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13">
         <v>42736</v>
       </c>
@@ -6919,7 +7090,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13">
         <v>42736</v>
       </c>
@@ -6982,13 +7153,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
@@ -6997,14 +7168,14 @@
     <col min="8" max="8" width="21.6640625" customWidth="1"/>
     <col min="9" max="9" width="21.6640625" style="14" customWidth="1"/>
     <col min="10" max="10" width="14.33203125" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" customWidth="1"/>
     <col min="13" max="13" width="28.6640625" customWidth="1"/>
     <col min="14" max="14" width="28.6640625" style="14" customWidth="1"/>
     <col min="15" max="15" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
@@ -7025,7 +7196,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:15" s="47" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="47" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="43"/>
       <c r="B2" s="43"/>
       <c r="C2" s="43" t="s">
@@ -7068,7 +7239,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -7115,7 +7286,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>42736</v>
       </c>
@@ -7152,7 +7323,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -7189,7 +7360,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>42736</v>
       </c>
@@ -7226,7 +7397,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -7263,7 +7434,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -7300,7 +7471,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="13">
         <v>42736</v>
       </c>
@@ -7337,7 +7508,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="13">
         <v>42736</v>
       </c>
@@ -7374,7 +7545,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13">
         <v>42736</v>
       </c>
@@ -7411,7 +7582,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13">
         <v>42736</v>
       </c>
@@ -7448,7 +7619,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13">
         <v>42736</v>
       </c>
@@ -7485,7 +7656,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13">
         <v>42736</v>
       </c>
@@ -7522,7 +7693,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13">
         <v>42736</v>
       </c>
@@ -7559,7 +7730,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13">
         <v>42736</v>
       </c>
@@ -7596,7 +7767,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13">
         <v>42736</v>
       </c>
@@ -7633,7 +7804,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13">
         <v>42736</v>
       </c>
@@ -7670,7 +7841,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="13">
         <v>42736</v>
       </c>
@@ -7707,7 +7878,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13">
         <v>42736</v>
       </c>
@@ -7744,7 +7915,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="13">
         <v>42736</v>
       </c>
@@ -7781,7 +7952,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="13">
         <v>42736</v>
       </c>
@@ -7818,7 +7989,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="13">
         <v>42736</v>
       </c>
@@ -7855,7 +8026,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="13">
         <v>42736</v>
       </c>
@@ -7892,7 +8063,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="13">
         <v>42736</v>
       </c>
@@ -7929,7 +8100,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="13">
         <v>42736</v>
       </c>
@@ -7966,7 +8137,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="13">
         <v>42736</v>
       </c>
@@ -8003,7 +8174,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="13">
         <v>42736</v>
       </c>
@@ -8040,7 +8211,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="13">
         <v>42736</v>
       </c>
@@ -8077,7 +8248,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="13">
         <v>42736</v>
       </c>
@@ -8114,7 +8285,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="13">
         <v>42736</v>
       </c>
@@ -8151,7 +8322,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="13">
         <v>42736</v>
       </c>
@@ -8188,7 +8359,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="13">
         <v>42736</v>
       </c>
@@ -8225,7 +8396,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="13">
         <v>42736</v>
       </c>
@@ -8262,7 +8433,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="13">
         <v>42736</v>
       </c>
@@ -8299,7 +8470,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="13">
         <v>42736</v>
       </c>
@@ -8336,7 +8507,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="13">
         <v>42736</v>
       </c>
@@ -8373,7 +8544,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="13">
         <v>42736</v>
       </c>
@@ -8410,7 +8581,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="13">
         <v>42736</v>
       </c>
@@ -8447,7 +8618,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="13">
         <v>42736</v>
       </c>
@@ -8484,7 +8655,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="13">
         <v>42736</v>
       </c>
@@ -8521,7 +8692,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="13">
         <v>42736</v>
       </c>
@@ -8558,7 +8729,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="13">
         <v>42736</v>
       </c>
@@ -8595,7 +8766,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="13">
         <v>42736</v>
       </c>
@@ -8632,7 +8803,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="13">
         <v>42736</v>
       </c>
@@ -8669,7 +8840,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="13">
         <v>42736</v>
       </c>
@@ -8706,7 +8877,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="13">
         <v>42736</v>
       </c>
@@ -8743,7 +8914,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="13">
         <v>42736</v>
       </c>
@@ -8780,7 +8951,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="13">
         <v>42736</v>
       </c>
@@ -8817,7 +8988,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="13">
         <v>42736</v>
       </c>
@@ -8854,7 +9025,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="13">
         <v>42736</v>
       </c>
@@ -8891,7 +9062,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="13">
         <v>42736</v>
       </c>
@@ -8928,7 +9099,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="13">
         <v>42736</v>
       </c>
@@ -8965,7 +9136,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="13">
         <v>42736</v>
       </c>
@@ -9002,7 +9173,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="13">
         <v>42736</v>
       </c>
@@ -9039,7 +9210,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="13">
         <v>42736</v>
       </c>
@@ -9076,7 +9247,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="13">
         <v>42736</v>
       </c>
@@ -9113,7 +9284,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="13">
         <v>42736</v>
       </c>
@@ -9150,7 +9321,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="13">
         <v>42736</v>
       </c>
@@ -9187,7 +9358,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="13">
         <v>42736</v>
       </c>
@@ -9224,7 +9395,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="13">
         <v>42736</v>
       </c>
@@ -9261,7 +9432,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="13">
         <v>42736</v>
       </c>
@@ -9298,7 +9469,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="13">
         <v>42736</v>
       </c>
@@ -9335,7 +9506,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="13">
         <v>42736</v>
       </c>
@@ -9372,7 +9543,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="13">
         <v>42736</v>
       </c>
@@ -9409,7 +9580,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="13">
         <v>42736</v>
       </c>
@@ -9446,7 +9617,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="13">
         <v>42736</v>
       </c>
@@ -9483,7 +9654,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="13">
         <v>42736</v>
       </c>
@@ -9520,7 +9691,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="13">
         <v>42736</v>
       </c>
@@ -9557,7 +9728,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="13">
         <v>42736</v>
       </c>
@@ -9594,7 +9765,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="13">
         <v>42736</v>
       </c>
@@ -9631,7 +9802,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="13">
         <v>42736</v>
       </c>
@@ -9668,7 +9839,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="13">
         <v>42736</v>
       </c>
@@ -9705,7 +9876,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="13">
         <v>42736</v>
       </c>
@@ -9742,7 +9913,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="13">
         <v>42736</v>
       </c>
@@ -9779,7 +9950,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="13">
         <v>42736</v>
       </c>
@@ -9816,7 +9987,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="13">
         <v>42736</v>
       </c>
@@ -9853,7 +10024,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="13">
         <v>42736</v>
       </c>
@@ -9890,7 +10061,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="13">
         <v>42736</v>
       </c>
@@ -9927,7 +10098,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="13">
         <v>42736</v>
       </c>
@@ -9964,7 +10135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="13">
         <v>42736</v>
       </c>
@@ -10001,7 +10172,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="13">
         <v>42736</v>
       </c>
@@ -10038,7 +10209,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="13">
         <v>42736</v>
       </c>
@@ -10075,7 +10246,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="13">
         <v>42736</v>
       </c>
@@ -10112,7 +10283,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="13">
         <v>42736</v>
       </c>
@@ -10149,7 +10320,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="13">
         <v>42736</v>
       </c>
@@ -10186,7 +10357,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="13">
         <v>42736</v>
       </c>
@@ -10223,7 +10394,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="13">
         <v>42736</v>
       </c>
@@ -10260,7 +10431,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="13">
         <v>42736</v>
       </c>
@@ -10297,7 +10468,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="13">
         <v>42736</v>
       </c>
@@ -10334,7 +10505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="13">
         <v>42736</v>
       </c>
@@ -10398,17 +10569,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.21875" customWidth="1"/>
+    <col min="3" max="3" width="30.1640625" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.21875" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -10424,7 +10595,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" s="30" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="30" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -10440,7 +10611,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -10460,7 +10631,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>42736</v>
       </c>
@@ -10478,7 +10649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -10515,7 +10686,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{00000000-0002-0000-0800-000003000000}">
           <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$34</xm:f>
+            <xm:f>CaseField!$D$4:$D$35</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D5</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
add case history tab component to ES (#329)
</commit_message>
<xml_diff>
--- a/aat/src/resource/CCD_CNP_27.xlsx
+++ b/aat/src/resource/CCD_CNP_27.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A533913\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/code/ccd/ccd-definition-store-api/aat/src/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{427A6C7C-B7FE-4CBA-907E-7C6E6F05AF53}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994F7540-D464-3047-B730-B47B7DA7E545}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2256" windowWidth="28800" windowHeight="15936" tabRatio="823" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1080" windowWidth="28800" windowHeight="15940" tabRatio="823" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1855" uniqueCount="275">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -862,6 +862,24 @@
   </si>
   <si>
     <t>Radio Value 2</t>
+  </si>
+  <si>
+    <t>HistoryComponentField</t>
+  </si>
+  <si>
+    <t>A `HistoryComponent` field</t>
+  </si>
+  <si>
+    <t>History tab component</t>
+  </si>
+  <si>
+    <t>CaseHistoryViewer</t>
+  </si>
+  <si>
+    <t>HistoryTab</t>
+  </si>
+  <si>
+    <t>History Tab</t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1096,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1101,6 +1119,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -1186,7 +1210,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1292,6 +1316,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="4" applyAlignment="1"/>
     <xf numFmtId="49" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1627,16 +1652,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" customWidth="1"/>
-    <col min="5" max="5" width="43.77734375" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="43.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1651,7 +1676,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -1664,7 +1689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -1681,7 +1706,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>42736</v>
       </c>
@@ -1723,17 +1748,17 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -1749,7 +1774,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" s="30" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="30" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -1765,7 +1790,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -1785,7 +1810,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
         <v>42736</v>
       </c>
@@ -1803,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="23">
         <v>42736</v>
       </c>
@@ -1821,7 +1846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23">
         <v>42736</v>
       </c>
@@ -1839,7 +1864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="23">
         <v>42736</v>
       </c>
@@ -1876,7 +1901,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0900-000004000000}">
           <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$34</xm:f>
+            <xm:f>CaseField!$D$4:$D$35</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D7</xm:sqref>
         </x14:dataValidation>
@@ -1897,18 +1922,18 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" style="70" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="71" customWidth="1"/>
-    <col min="3" max="3" width="29.77734375" style="71" customWidth="1"/>
-    <col min="4" max="4" width="19.77734375" style="71" customWidth="1"/>
-    <col min="5" max="5" width="20.21875" style="71" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" style="70" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="71" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" style="71" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" style="71" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="71" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" style="71" customWidth="1"/>
-    <col min="7" max="16384" width="8.77734375" style="14"/>
+    <col min="7" max="16384" width="8.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="62" t="s">
         <v>130</v>
       </c>
@@ -1924,7 +1949,7 @@
       <c r="E1" s="66"/>
       <c r="F1" s="66"/>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="48" x14ac:dyDescent="0.15">
       <c r="A2" s="67"/>
       <c r="B2" s="67"/>
       <c r="C2" s="68" t="s">
@@ -1940,7 +1965,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="69" t="s">
         <v>8</v>
       </c>
@@ -1960,7 +1985,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>42736</v>
       </c>
@@ -1978,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -2015,7 +2040,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{00000000-0002-0000-0A00-000003000000}">
           <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$34</xm:f>
+            <xm:f>CaseField!$D$4:$D$35</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D5</xm:sqref>
         </x14:dataValidation>
@@ -2036,7 +2061,7 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -2046,7 +2071,7 @@
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -2062,7 +2087,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" s="30" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="30" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
       <c r="C2" s="31" t="s">
@@ -2078,7 +2103,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -2098,7 +2123,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
         <v>42736</v>
       </c>
@@ -2116,7 +2141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="23">
         <v>42736</v>
       </c>
@@ -2134,7 +2159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23">
         <v>42736</v>
       </c>
@@ -2152,7 +2177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="23">
         <v>42736</v>
       </c>
@@ -2189,7 +2214,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field id" xr:uid="{00000000-0002-0000-0B00-000004000000}">
           <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$34</xm:f>
+            <xm:f>CaseField!$D$4:$D$35</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D7</xm:sqref>
         </x14:dataValidation>
@@ -2204,25 +2229,25 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" customWidth="1"/>
     <col min="4" max="4" width="31.6640625" customWidth="1"/>
     <col min="5" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="16.33203125" customWidth="1"/>
-    <col min="8" max="8" width="40.77734375" customWidth="1"/>
+    <col min="8" max="8" width="40.83203125" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -2241,7 +2266,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
       <c r="C2" s="31" t="s">
@@ -2266,7 +2291,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -2295,7 +2320,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25">
         <v>42736</v>
       </c>
@@ -2322,7 +2347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27">
         <v>42736</v>
       </c>
@@ -2349,7 +2374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27">
         <v>42736</v>
       </c>
@@ -2376,7 +2401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27">
         <v>42736</v>
       </c>
@@ -2403,7 +2428,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27">
         <v>42736</v>
       </c>
@@ -2430,7 +2455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27">
         <v>42736</v>
       </c>
@@ -2457,7 +2482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27">
         <v>42736</v>
       </c>
@@ -2484,7 +2509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27">
         <v>42736</v>
       </c>
@@ -2511,7 +2536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27">
         <v>42736</v>
       </c>
@@ -2538,7 +2563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27">
         <v>42736</v>
       </c>
@@ -2565,7 +2590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="27">
         <v>42736</v>
       </c>
@@ -2592,7 +2617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="27">
         <v>42736</v>
       </c>
@@ -2619,7 +2644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27">
         <v>42736</v>
       </c>
@@ -2646,7 +2671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27">
         <v>42736</v>
       </c>
@@ -2673,7 +2698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="27">
         <v>42736</v>
       </c>
@@ -2700,7 +2725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="27">
         <v>42736</v>
       </c>
@@ -2727,34 +2752,34 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="27">
         <v>42736</v>
       </c>
       <c r="B20" s="27"/>
       <c r="C20" s="14" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="D20" s="28" t="s">
         <v>56</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>211</v>
+        <v>273</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>212</v>
+        <v>274</v>
       </c>
       <c r="G20" s="28">
-        <v>1</v>
-      </c>
-      <c r="H20" s="28" t="s">
-        <v>135</v>
+        <v>4</v>
+      </c>
+      <c r="H20" s="42" t="s">
+        <v>269</v>
       </c>
       <c r="I20" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="27">
         <v>42736</v>
       </c>
@@ -2775,13 +2800,13 @@
         <v>1</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I21" s="28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="27">
         <v>42736</v>
       </c>
@@ -2802,13 +2827,13 @@
         <v>1</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I22" s="28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="27">
         <v>42736</v>
       </c>
@@ -2828,14 +2853,14 @@
       <c r="G23" s="28">
         <v>1</v>
       </c>
-      <c r="H23" s="42" t="s">
-        <v>144</v>
+      <c r="H23" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="I23" s="28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27">
         <v>42736</v>
       </c>
@@ -2856,13 +2881,13 @@
         <v>1</v>
       </c>
       <c r="H24" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I24" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="27">
         <v>42736</v>
       </c>
@@ -2874,22 +2899,22 @@
         <v>56</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G25" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H25" s="42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I25" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27">
         <v>42736</v>
       </c>
@@ -2910,13 +2935,13 @@
         <v>2</v>
       </c>
       <c r="H26" s="42" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="I26" s="28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="27">
         <v>42736</v>
       </c>
@@ -2937,13 +2962,13 @@
         <v>2</v>
       </c>
       <c r="H27" s="42" t="s">
-        <v>247</v>
+        <v>158</v>
       </c>
       <c r="I27" s="28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="27">
         <v>42736</v>
       </c>
@@ -2964,13 +2989,13 @@
         <v>2</v>
       </c>
       <c r="H28" s="42" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="I28" s="28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="27">
         <v>42736</v>
       </c>
@@ -2991,13 +3016,13 @@
         <v>2</v>
       </c>
       <c r="H29" s="42" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I29" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="27">
         <v>42736</v>
       </c>
@@ -3018,13 +3043,13 @@
         <v>2</v>
       </c>
       <c r="H30" s="42" t="s">
-        <v>258</v>
+        <v>160</v>
       </c>
       <c r="I30" s="28">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="27">
         <v>42736</v>
       </c>
@@ -3045,13 +3070,13 @@
         <v>2</v>
       </c>
       <c r="H31" s="42" t="s">
-        <v>170</v>
+        <v>258</v>
       </c>
       <c r="I31" s="28">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="27">
         <v>42736</v>
       </c>
@@ -3063,22 +3088,22 @@
         <v>56</v>
       </c>
       <c r="E32" s="42" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="G32" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H32" s="42" t="s">
-        <v>225</v>
+        <v>170</v>
       </c>
       <c r="I32" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="27">
         <v>42736</v>
       </c>
@@ -3099,13 +3124,13 @@
         <v>3</v>
       </c>
       <c r="H33" s="42" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="I33" s="28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="27">
         <v>42736</v>
       </c>
@@ -3126,21 +3151,75 @@
         <v>3</v>
       </c>
       <c r="H34" s="42" t="s">
+        <v>240</v>
+      </c>
+      <c r="I34" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="27">
+        <v>42736</v>
+      </c>
+      <c r="B35" s="27"/>
+      <c r="C35" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="G35" s="28">
+        <v>3</v>
+      </c>
+      <c r="H35" s="42" t="s">
         <v>243</v>
       </c>
-      <c r="I34" s="28">
+      <c r="I35" s="28">
         <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="27">
+        <v>42736</v>
+      </c>
+      <c r="B36" s="27"/>
+      <c r="C36" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>274</v>
+      </c>
+      <c r="G36" s="28">
+        <v>4</v>
+      </c>
+      <c r="H36" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="I36" s="28">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="I4:I34 G4:G34" xr:uid="{00000000-0002-0000-0C00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G36 I4:I36" xr:uid="{00000000-0002-0000-0C00-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A34" xr:uid="{00000000-0002-0000-0C00-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A36" xr:uid="{00000000-0002-0000-0C00-000002000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B34" xr:uid="{00000000-0002-0000-0C00-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B36" xr:uid="{00000000-0002-0000-0C00-000000000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -3162,17 +3241,17 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="28.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
@@ -3187,7 +3266,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="3" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="37" t="s">
         <v>8</v>
       </c>
@@ -3207,7 +3286,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="72">
         <v>42736</v>
       </c>
@@ -3246,15 +3325,15 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -3269,7 +3348,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" s="30" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="30" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
       <c r="C2" s="31" t="s">
@@ -3282,7 +3361,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -3299,7 +3378,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="29">
         <v>42736</v>
       </c>
@@ -3314,7 +3393,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="14" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="29">
         <v>42736</v>
       </c>
@@ -3348,18 +3427,18 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.21875" style="61" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="61" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" style="61" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" style="61" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="61" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="61" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" style="61" customWidth="1"/>
     <col min="5" max="5" width="27" style="61" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" style="61" customWidth="1"/>
-    <col min="7" max="16384" width="8.77734375" style="54"/>
+    <col min="6" max="6" width="14.5" style="61" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="49" t="s">
         <v>128</v>
       </c>
@@ -3375,7 +3454,7 @@
       <c r="E1" s="53"/>
       <c r="F1" s="53"/>
     </row>
-    <row r="2" spans="1:6" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="55"/>
       <c r="B2" s="55"/>
       <c r="C2" s="56" t="s">
@@ -3391,7 +3470,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="57" t="s">
         <v>8</v>
       </c>
@@ -3411,7 +3490,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="59">
         <v>42736</v>
       </c>
@@ -3429,7 +3508,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="59">
         <v>42736</v>
       </c>
@@ -3447,7 +3526,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="59">
         <v>42736</v>
       </c>
@@ -3465,7 +3544,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="59">
         <v>42736</v>
       </c>
@@ -3483,7 +3562,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="59">
         <v>42736</v>
       </c>
@@ -3501,7 +3580,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="59">
         <v>42736</v>
       </c>
@@ -3538,16 +3617,16 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.77734375" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
@@ -3563,7 +3642,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" s="30" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="30" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -3579,7 +3658,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="33" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -3599,7 +3678,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="72">
         <v>42736</v>
       </c>
@@ -3616,7 +3695,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="72">
         <v>42736</v>
       </c>
@@ -3633,7 +3712,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="72">
         <v>42736</v>
       </c>
@@ -3650,7 +3729,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="72">
         <v>42736</v>
       </c>
@@ -3667,7 +3746,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="72">
         <v>42736</v>
       </c>
@@ -3684,7 +3763,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="72">
         <v>42736</v>
       </c>
@@ -3701,7 +3780,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="72">
         <v>42736</v>
       </c>
@@ -3718,7 +3797,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="72">
         <v>42736</v>
       </c>
@@ -3735,7 +3814,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="72">
         <v>42736</v>
       </c>
@@ -3752,7 +3831,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="72">
         <v>42736</v>
       </c>
@@ -3769,7 +3848,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="72">
         <v>42736</v>
       </c>
@@ -3786,7 +3865,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="72">
         <v>42736</v>
       </c>
@@ -3816,22 +3895,22 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
@@ -3846,7 +3925,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="70" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -3862,7 +3941,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="33" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -3882,7 +3961,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="72">
         <v>42736</v>
       </c>
@@ -3899,7 +3978,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="72">
         <v>42736</v>
       </c>
@@ -3916,7 +3995,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="72">
         <v>42736</v>
       </c>
@@ -3933,7 +4012,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="72">
         <v>42736</v>
       </c>
@@ -3950,7 +4029,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="72">
         <v>42736</v>
       </c>
@@ -3967,7 +4046,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="72">
         <v>42736</v>
       </c>
@@ -3984,7 +4063,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="72">
         <v>42736</v>
       </c>
@@ -4001,7 +4080,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="72">
         <v>42736</v>
       </c>
@@ -4018,7 +4097,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="72">
         <v>42736</v>
       </c>
@@ -4035,7 +4114,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="72">
         <v>42736</v>
       </c>
@@ -4052,7 +4131,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="72">
         <v>42736</v>
       </c>
@@ -4069,7 +4148,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="72">
         <v>42736</v>
       </c>
@@ -4086,7 +4165,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="72">
         <v>42736</v>
       </c>
@@ -4104,7 +4183,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="72">
         <v>42736</v>
       </c>
@@ -4121,7 +4200,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="72">
         <v>42736</v>
       </c>
@@ -4139,7 +4218,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="72">
         <v>42736</v>
       </c>
@@ -4156,15 +4235,15 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="72">
         <v>42736</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>135</v>
+        <v>234</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>269</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>236</v>
@@ -4173,7 +4252,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="72">
         <v>42736</v>
       </c>
@@ -4181,7 +4260,7 @@
         <v>251</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>236</v>
@@ -4190,7 +4269,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="72">
         <v>42736</v>
       </c>
@@ -4198,7 +4277,7 @@
         <v>251</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>236</v>
@@ -4207,15 +4286,15 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="72">
         <v>42736</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="D23" s="42" t="s">
-        <v>144</v>
+      <c r="D23" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>236</v>
@@ -4224,7 +4303,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="72">
         <v>42736</v>
       </c>
@@ -4232,7 +4311,7 @@
         <v>251</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>236</v>
@@ -4241,7 +4320,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="72">
         <v>42736</v>
       </c>
@@ -4249,7 +4328,7 @@
         <v>251</v>
       </c>
       <c r="D25" s="42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E25" s="14" t="s">
         <v>236</v>
@@ -4258,7 +4337,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="72">
         <v>42736</v>
       </c>
@@ -4266,7 +4345,7 @@
         <v>251</v>
       </c>
       <c r="D26" s="42" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>236</v>
@@ -4275,7 +4354,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="72">
         <v>42736</v>
       </c>
@@ -4283,7 +4362,7 @@
         <v>251</v>
       </c>
       <c r="D27" s="42" t="s">
-        <v>247</v>
+        <v>158</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>236</v>
@@ -4292,7 +4371,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="72">
         <v>42736</v>
       </c>
@@ -4300,7 +4379,7 @@
         <v>251</v>
       </c>
       <c r="D28" s="42" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>236</v>
@@ -4309,7 +4388,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="72">
         <v>42736</v>
       </c>
@@ -4317,7 +4396,7 @@
         <v>251</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>236</v>
@@ -4326,7 +4405,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="72">
         <v>42736</v>
       </c>
@@ -4334,7 +4413,7 @@
         <v>251</v>
       </c>
       <c r="D30" s="42" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>236</v>
@@ -4343,15 +4422,15 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="72">
         <v>42736</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="D31" s="24" t="s">
-        <v>243</v>
+      <c r="D31" s="42" t="s">
+        <v>170</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>236</v>
@@ -4360,15 +4439,15 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="72">
         <v>42736</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="D32" s="42" t="s">
-        <v>240</v>
+      <c r="D32" s="24" t="s">
+        <v>243</v>
       </c>
       <c r="E32" s="14" t="s">
         <v>236</v>
@@ -4377,7 +4456,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="72">
         <v>42736</v>
       </c>
@@ -4385,7 +4464,7 @@
         <v>251</v>
       </c>
       <c r="D33" s="42" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="E33" s="14" t="s">
         <v>236</v>
@@ -4394,7 +4473,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="72">
         <v>42736</v>
       </c>
@@ -4402,12 +4481,46 @@
         <v>251</v>
       </c>
       <c r="D34" s="42" t="s">
-        <v>258</v>
+        <v>225</v>
       </c>
       <c r="E34" s="14" t="s">
         <v>236</v>
       </c>
       <c r="F34" s="24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="72">
+        <v>42736</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="72">
+        <v>42736</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="F36" s="24" t="s">
         <v>124</v>
       </c>
     </row>
@@ -4430,20 +4543,20 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.77734375" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -4462,7 +4575,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" s="30" customFormat="1" ht="73.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="30" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -4487,7 +4600,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -4516,7 +4629,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="11">
         <v>42736</v>
       </c>
@@ -4537,7 +4650,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -4579,28 +4692,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.77734375" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" customWidth="1"/>
     <col min="4" max="4" width="41.33203125" customWidth="1"/>
-    <col min="5" max="5" width="40.77734375" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" customWidth="1"/>
+    <col min="5" max="5" width="40.83203125" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
     <col min="7" max="8" width="37" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="10" max="10" width="20.33203125" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="13" width="8.77734375" customWidth="1"/>
+    <col min="12" max="13" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4620,7 +4733,7 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:13" s="30" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="30" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -4653,7 +4766,7 @@
       <c r="L2" s="32"/>
       <c r="M2" s="32"/>
     </row>
-    <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -4694,7 +4807,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>42736</v>
       </c>
@@ -4723,7 +4836,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -4752,7 +4865,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>42736</v>
       </c>
@@ -4781,7 +4894,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -4810,7 +4923,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -4839,7 +4952,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="13">
         <v>42736</v>
       </c>
@@ -4868,7 +4981,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="13">
         <v>42736</v>
       </c>
@@ -4897,7 +5010,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13">
         <v>42736</v>
       </c>
@@ -4926,7 +5039,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13">
         <v>42736</v>
       </c>
@@ -4955,7 +5068,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13">
         <v>42736</v>
       </c>
@@ -4986,7 +5099,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13">
         <v>42736</v>
       </c>
@@ -5017,7 +5130,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13">
         <v>42736</v>
       </c>
@@ -5048,7 +5161,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13">
         <v>42736</v>
       </c>
@@ -5077,7 +5190,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13">
         <v>42736</v>
       </c>
@@ -5106,7 +5219,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13">
         <v>42736</v>
       </c>
@@ -5135,7 +5248,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="13">
         <v>42736</v>
       </c>
@@ -5166,27 +5279,27 @@
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13">
         <v>42736</v>
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="F20" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="G20" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="H20" s="28"/>
+        <v>234</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="F20" s="42" t="s">
+        <v>271</v>
+      </c>
+      <c r="G20" s="75" t="s">
+        <v>272</v>
+      </c>
+      <c r="H20" s="42"/>
       <c r="I20" s="28" t="s">
         <v>26</v>
       </c>
@@ -5195,7 +5308,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="13">
         <v>42736</v>
       </c>
@@ -5204,16 +5317,16 @@
         <v>251</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H21" s="28"/>
       <c r="I21" s="28" t="s">
@@ -5224,7 +5337,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="13">
         <v>42736</v>
       </c>
@@ -5233,16 +5346,16 @@
         <v>251</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="G22" s="42" t="s">
-        <v>30</v>
+        <v>142</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>28</v>
       </c>
       <c r="H22" s="28"/>
       <c r="I22" s="28" t="s">
@@ -5253,7 +5366,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="13">
         <v>42736</v>
       </c>
@@ -5261,17 +5374,17 @@
       <c r="C23" s="28" t="s">
         <v>251</v>
       </c>
-      <c r="D23" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="E23" s="42" t="s">
-        <v>145</v>
-      </c>
-      <c r="F23" s="42" t="s">
-        <v>148</v>
+      <c r="D23" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>141</v>
       </c>
       <c r="G23" s="42" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="H23" s="28"/>
       <c r="I23" s="28" t="s">
@@ -5282,7 +5395,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="13">
         <v>42736</v>
       </c>
@@ -5291,16 +5404,16 @@
         <v>251</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F24" s="42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G24" s="42" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="H24" s="28"/>
       <c r="I24" s="28" t="s">
@@ -5311,7 +5424,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="13">
         <v>42736</v>
       </c>
@@ -5320,16 +5433,16 @@
         <v>251</v>
       </c>
       <c r="D25" s="42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F25" s="42" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G25" s="42" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="H25" s="28"/>
       <c r="I25" s="28" t="s">
@@ -5340,7 +5453,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="13">
         <v>42736</v>
       </c>
@@ -5349,16 +5462,16 @@
         <v>251</v>
       </c>
       <c r="D26" s="42" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="E26" s="42" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F26" s="42" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G26" s="42" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="H26" s="28"/>
       <c r="I26" s="28" t="s">
@@ -5369,7 +5482,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="13">
         <v>42736</v>
       </c>
@@ -5378,16 +5491,16 @@
         <v>251</v>
       </c>
       <c r="D27" s="42" t="s">
-        <v>247</v>
+        <v>158</v>
       </c>
       <c r="E27" s="42" t="s">
-        <v>248</v>
+        <v>153</v>
       </c>
       <c r="F27" s="42" t="s">
-        <v>249</v>
+        <v>154</v>
       </c>
       <c r="G27" s="42" t="s">
-        <v>250</v>
+        <v>27</v>
       </c>
       <c r="H27" s="28"/>
       <c r="I27" s="28" t="s">
@@ -5398,7 +5511,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="13">
         <v>42736</v>
       </c>
@@ -5407,16 +5520,16 @@
         <v>251</v>
       </c>
       <c r="D28" s="42" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>157</v>
+        <v>248</v>
       </c>
       <c r="F28" s="42" t="s">
-        <v>159</v>
+        <v>249</v>
       </c>
       <c r="G28" s="42" t="s">
-        <v>155</v>
+        <v>250</v>
       </c>
       <c r="H28" s="28"/>
       <c r="I28" s="28" t="s">
@@ -5427,7 +5540,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="13">
         <v>42736</v>
       </c>
@@ -5436,20 +5549,18 @@
         <v>251</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F29" s="42" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G29" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="H29" s="42" t="s">
-        <v>163</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="H29" s="28"/>
       <c r="I29" s="28" t="s">
         <v>26</v>
       </c>
@@ -5458,7 +5569,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="13">
         <v>42736</v>
       </c>
@@ -5467,19 +5578,19 @@
         <v>251</v>
       </c>
       <c r="D30" s="42" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E30" s="42" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="F30" s="42" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G30" s="42" t="s">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="H30" s="42" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="I30" s="28" t="s">
         <v>26</v>
@@ -5489,7 +5600,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="13">
         <v>42736</v>
       </c>
@@ -5498,19 +5609,19 @@
         <v>251</v>
       </c>
       <c r="D31" s="42" t="s">
-        <v>240</v>
+        <v>170</v>
       </c>
       <c r="E31" s="42" t="s">
-        <v>241</v>
+        <v>171</v>
       </c>
       <c r="F31" s="42" t="s">
-        <v>242</v>
+        <v>172</v>
       </c>
       <c r="G31" s="42" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="H31" s="42" t="s">
-        <v>25</v>
+        <v>173</v>
       </c>
       <c r="I31" s="28" t="s">
         <v>26</v>
@@ -5520,7 +5631,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="13">
         <v>42736</v>
       </c>
@@ -5529,18 +5640,20 @@
         <v>251</v>
       </c>
       <c r="D32" s="42" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="E32" s="42" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
       <c r="F32" s="42" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="G32" s="42" t="s">
-        <v>228</v>
-      </c>
-      <c r="H32" s="42"/>
+        <v>80</v>
+      </c>
+      <c r="H32" s="42" t="s">
+        <v>25</v>
+      </c>
       <c r="I32" s="28" t="s">
         <v>26</v>
       </c>
@@ -5549,7 +5662,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="13">
         <v>42736</v>
       </c>
@@ -5558,16 +5671,16 @@
         <v>251</v>
       </c>
       <c r="D33" s="42" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="E33" s="42" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="F33" s="42" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="G33" s="42" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="H33" s="42"/>
       <c r="I33" s="28" t="s">
@@ -5578,7 +5691,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="13">
         <v>42736</v>
       </c>
@@ -5587,20 +5700,18 @@
         <v>251</v>
       </c>
       <c r="D34" s="42" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="E34" s="42" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="F34" s="42" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="G34" s="42" t="s">
-        <v>261</v>
-      </c>
-      <c r="H34" s="42" t="s">
-        <v>262</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="H34" s="42"/>
       <c r="I34" s="28" t="s">
         <v>26</v>
       </c>
@@ -5609,12 +5720,72 @@
         <v>117</v>
       </c>
     </row>
+    <row r="35" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="E35" s="42" t="s">
+        <v>259</v>
+      </c>
+      <c r="F35" s="42" t="s">
+        <v>260</v>
+      </c>
+      <c r="G35" s="42" t="s">
+        <v>261</v>
+      </c>
+      <c r="H35" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="I35" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B36" s="13"/>
+      <c r="C36" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="F36" s="42" t="s">
+        <v>271</v>
+      </c>
+      <c r="G36" s="75" t="s">
+        <v>272</v>
+      </c>
+      <c r="H36" s="42"/>
+      <c r="I36" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J36" s="28"/>
+      <c r="K36" s="28" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A34" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A36" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B34" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B36" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -5636,15 +5807,15 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="31.6640625" customWidth="1"/>
     <col min="5" max="5" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -5659,7 +5830,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -5672,7 +5843,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -5689,7 +5860,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="15">
         <v>42736</v>
       </c>
@@ -5704,7 +5875,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="15">
         <v>42736</v>
       </c>
@@ -5719,7 +5890,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="15">
         <v>42736</v>
       </c>
@@ -5734,7 +5905,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="15">
         <v>42736</v>
       </c>
@@ -5749,7 +5920,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="15">
         <v>42736</v>
       </c>
@@ -5764,7 +5935,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="15">
         <v>42736</v>
       </c>
@@ -5779,7 +5950,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="15">
         <v>42736</v>
       </c>
@@ -5794,7 +5965,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="15">
         <v>42736</v>
       </c>
@@ -5809,7 +5980,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="15">
         <v>42736</v>
       </c>
@@ -5824,7 +5995,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="15">
         <v>42736</v>
       </c>
@@ -5839,7 +6010,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="15">
         <v>42736</v>
       </c>
@@ -5880,7 +6051,7 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -5889,15 +6060,15 @@
     <col min="5" max="5" width="28.33203125" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="24.77734375" customWidth="1"/>
-    <col min="9" max="9" width="24.77734375" style="14" customWidth="1"/>
+    <col min="8" max="8" width="24.83203125" customWidth="1"/>
+    <col min="9" max="9" width="24.83203125" style="14" customWidth="1"/>
     <col min="10" max="10" width="37" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
-    <col min="13" max="14" width="8.77734375" customWidth="1"/>
+    <col min="13" max="14" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -5918,7 +6089,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -5954,7 +6125,7 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -5998,7 +6169,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>42736</v>
       </c>
@@ -6028,7 +6199,7 @@
       <c r="M4" s="35"/>
       <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -6060,7 +6231,7 @@
       <c r="M5" s="35"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="11">
         <v>42736</v>
       </c>
@@ -6088,7 +6259,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -6118,7 +6289,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -6172,18 +6343,18 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.33203125" customWidth="1"/>
     <col min="5" max="5" width="31.6640625" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -6200,7 +6371,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" ht="61.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="61" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -6213,7 +6384,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -6236,7 +6407,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="11">
         <v>42736</v>
       </c>
@@ -6255,7 +6426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -6274,7 +6445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>42736</v>
       </c>
@@ -6293,7 +6464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -6312,7 +6483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -6331,7 +6502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="13">
         <v>42736</v>
       </c>
@@ -6380,11 +6551,11 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.6640625" customWidth="1"/>
     <col min="6" max="6" width="45.33203125" customWidth="1"/>
@@ -6394,14 +6565,14 @@
     <col min="10" max="10" width="29.6640625" style="30" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="32" style="30" customWidth="1"/>
     <col min="12" max="12" width="31.33203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.77734375" style="30" customWidth="1"/>
+    <col min="13" max="13" width="29.83203125" style="30" customWidth="1"/>
     <col min="14" max="14" width="26.6640625" style="30" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="29.33203125" style="30" customWidth="1"/>
     <col min="16" max="16" width="23.6640625" customWidth="1"/>
-    <col min="17" max="17" width="31.21875" customWidth="1"/>
+    <col min="17" max="17" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -6420,7 +6591,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -6469,7 +6640,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -6522,7 +6693,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="11">
         <v>42736</v>
       </c>
@@ -6551,7 +6722,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -6588,7 +6759,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>42736</v>
       </c>
@@ -6625,7 +6796,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -6662,7 +6833,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -6699,7 +6870,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="13">
         <v>42736</v>
       </c>
@@ -6736,7 +6907,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="13">
         <v>42736</v>
       </c>
@@ -6771,7 +6942,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13">
         <v>42736</v>
       </c>
@@ -6808,7 +6979,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13">
         <v>42736</v>
       </c>
@@ -6845,7 +7016,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13">
         <v>42736</v>
       </c>
@@ -6882,7 +7053,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13">
         <v>42736</v>
       </c>
@@ -6919,7 +7090,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13">
         <v>42736</v>
       </c>
@@ -6982,13 +7153,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
@@ -6997,14 +7168,14 @@
     <col min="8" max="8" width="21.6640625" customWidth="1"/>
     <col min="9" max="9" width="21.6640625" style="14" customWidth="1"/>
     <col min="10" max="10" width="14.33203125" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" customWidth="1"/>
     <col min="13" max="13" width="28.6640625" customWidth="1"/>
     <col min="14" max="14" width="28.6640625" style="14" customWidth="1"/>
     <col min="15" max="15" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
@@ -7025,7 +7196,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:15" s="47" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="47" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="43"/>
       <c r="B2" s="43"/>
       <c r="C2" s="43" t="s">
@@ -7068,7 +7239,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -7115,7 +7286,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="13">
         <v>42736</v>
       </c>
@@ -7152,7 +7323,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -7189,7 +7360,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>42736</v>
       </c>
@@ -7226,7 +7397,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -7263,7 +7434,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -7300,7 +7471,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="13">
         <v>42736</v>
       </c>
@@ -7337,7 +7508,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="13">
         <v>42736</v>
       </c>
@@ -7374,7 +7545,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13">
         <v>42736</v>
       </c>
@@ -7411,7 +7582,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13">
         <v>42736</v>
       </c>
@@ -7448,7 +7619,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13">
         <v>42736</v>
       </c>
@@ -7485,7 +7656,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13">
         <v>42736</v>
       </c>
@@ -7522,7 +7693,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13">
         <v>42736</v>
       </c>
@@ -7559,7 +7730,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13">
         <v>42736</v>
       </c>
@@ -7596,7 +7767,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13">
         <v>42736</v>
       </c>
@@ -7633,7 +7804,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13">
         <v>42736</v>
       </c>
@@ -7670,7 +7841,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="13">
         <v>42736</v>
       </c>
@@ -7707,7 +7878,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13">
         <v>42736</v>
       </c>
@@ -7744,7 +7915,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="13">
         <v>42736</v>
       </c>
@@ -7781,7 +7952,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="13">
         <v>42736</v>
       </c>
@@ -7818,7 +7989,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="13">
         <v>42736</v>
       </c>
@@ -7855,7 +8026,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="13">
         <v>42736</v>
       </c>
@@ -7892,7 +8063,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="13">
         <v>42736</v>
       </c>
@@ -7929,7 +8100,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="13">
         <v>42736</v>
       </c>
@@ -7966,7 +8137,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="13">
         <v>42736</v>
       </c>
@@ -8003,7 +8174,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="13">
         <v>42736</v>
       </c>
@@ -8040,7 +8211,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="13">
         <v>42736</v>
       </c>
@@ -8077,7 +8248,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="13">
         <v>42736</v>
       </c>
@@ -8114,7 +8285,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="13">
         <v>42736</v>
       </c>
@@ -8151,7 +8322,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="13">
         <v>42736</v>
       </c>
@@ -8188,7 +8359,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="13">
         <v>42736</v>
       </c>
@@ -8225,7 +8396,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="13">
         <v>42736</v>
       </c>
@@ -8262,7 +8433,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="13">
         <v>42736</v>
       </c>
@@ -8299,7 +8470,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="13">
         <v>42736</v>
       </c>
@@ -8336,7 +8507,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="13">
         <v>42736</v>
       </c>
@@ -8373,7 +8544,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="13">
         <v>42736</v>
       </c>
@@ -8410,7 +8581,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="13">
         <v>42736</v>
       </c>
@@ -8447,7 +8618,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="13">
         <v>42736</v>
       </c>
@@ -8484,7 +8655,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="13">
         <v>42736</v>
       </c>
@@ -8521,7 +8692,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="13">
         <v>42736</v>
       </c>
@@ -8558,7 +8729,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="13">
         <v>42736</v>
       </c>
@@ -8595,7 +8766,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="13">
         <v>42736</v>
       </c>
@@ -8632,7 +8803,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="13">
         <v>42736</v>
       </c>
@@ -8669,7 +8840,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="13">
         <v>42736</v>
       </c>
@@ -8706,7 +8877,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="13">
         <v>42736</v>
       </c>
@@ -8743,7 +8914,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="13">
         <v>42736</v>
       </c>
@@ -8780,7 +8951,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="13">
         <v>42736</v>
       </c>
@@ -8817,7 +8988,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="13">
         <v>42736</v>
       </c>
@@ -8854,7 +9025,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="13">
         <v>42736</v>
       </c>
@@ -8891,7 +9062,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="13">
         <v>42736</v>
       </c>
@@ -8928,7 +9099,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="13">
         <v>42736</v>
       </c>
@@ -8965,7 +9136,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="13">
         <v>42736</v>
       </c>
@@ -9002,7 +9173,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="13">
         <v>42736</v>
       </c>
@@ -9039,7 +9210,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="13">
         <v>42736</v>
       </c>
@@ -9076,7 +9247,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="13">
         <v>42736</v>
       </c>
@@ -9113,7 +9284,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="13">
         <v>42736</v>
       </c>
@@ -9150,7 +9321,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="13">
         <v>42736</v>
       </c>
@@ -9187,7 +9358,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="13">
         <v>42736</v>
       </c>
@@ -9224,7 +9395,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="13">
         <v>42736</v>
       </c>
@@ -9261,7 +9432,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="13">
         <v>42736</v>
       </c>
@@ -9298,7 +9469,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="13">
         <v>42736</v>
       </c>
@@ -9335,7 +9506,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="13">
         <v>42736</v>
       </c>
@@ -9372,7 +9543,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="13">
         <v>42736</v>
       </c>
@@ -9409,7 +9580,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="13">
         <v>42736</v>
       </c>
@@ -9446,7 +9617,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="13">
         <v>42736</v>
       </c>
@@ -9483,7 +9654,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="13">
         <v>42736</v>
       </c>
@@ -9520,7 +9691,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="13">
         <v>42736</v>
       </c>
@@ -9557,7 +9728,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="13">
         <v>42736</v>
       </c>
@@ -9594,7 +9765,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="13">
         <v>42736</v>
       </c>
@@ -9631,7 +9802,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="13">
         <v>42736</v>
       </c>
@@ -9668,7 +9839,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="13">
         <v>42736</v>
       </c>
@@ -9705,7 +9876,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="13">
         <v>42736</v>
       </c>
@@ -9742,7 +9913,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="13">
         <v>42736</v>
       </c>
@@ -9779,7 +9950,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="13">
         <v>42736</v>
       </c>
@@ -9816,7 +9987,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="13">
         <v>42736</v>
       </c>
@@ -9853,7 +10024,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="13">
         <v>42736</v>
       </c>
@@ -9890,7 +10061,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="13">
         <v>42736</v>
       </c>
@@ -9927,7 +10098,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="13">
         <v>42736</v>
       </c>
@@ -9964,7 +10135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="13">
         <v>42736</v>
       </c>
@@ -10001,7 +10172,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="13">
         <v>42736</v>
       </c>
@@ -10038,7 +10209,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="13">
         <v>42736</v>
       </c>
@@ -10075,7 +10246,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="13">
         <v>42736</v>
       </c>
@@ -10112,7 +10283,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="13">
         <v>42736</v>
       </c>
@@ -10149,7 +10320,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="13">
         <v>42736</v>
       </c>
@@ -10186,7 +10357,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="13">
         <v>42736</v>
       </c>
@@ -10223,7 +10394,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="13">
         <v>42736</v>
       </c>
@@ -10260,7 +10431,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="13">
         <v>42736</v>
       </c>
@@ -10297,7 +10468,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="13">
         <v>42736</v>
       </c>
@@ -10334,7 +10505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="13">
         <v>42736</v>
       </c>
@@ -10398,17 +10569,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.21875" customWidth="1"/>
+    <col min="3" max="3" width="30.1640625" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.21875" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -10424,7 +10595,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" s="30" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="30" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -10440,7 +10611,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -10460,7 +10631,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>42736</v>
       </c>
@@ -10478,7 +10649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -10515,7 +10686,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a valid field type" xr:uid="{00000000-0002-0000-0800-000003000000}">
           <x14:formula1>
-            <xm:f>CaseField!$D$4:$D$34</xm:f>
+            <xm:f>CaseField!$D$4:$D$35</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D5</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
RDM-4362 added new tab definition for Case Tab per role functional tests
</commit_message>
<xml_diff>
--- a/aat/src/resource/CCD_CNP_27.xlsx
+++ b/aat/src/resource/CCD_CNP_27.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/code/ccd/ccd-definition-store-api/aat/src/resource/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/space/workspace/ccd-definition-store-api/aat/src/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994F7540-D464-3047-B730-B47B7DA7E545}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA53374-0933-8745-87CA-44EC347A41DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="28800" windowHeight="15940" tabRatio="823" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1620" windowWidth="28800" windowHeight="15940" tabRatio="823" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1855" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1878" uniqueCount="279">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -880,6 +880,18 @@
   </si>
   <si>
     <t>History Tab</t>
+  </si>
+  <si>
+    <t>FourthTab</t>
+  </si>
+  <si>
+    <t>Fourth Tab</t>
+  </si>
+  <si>
+    <t>MaxLength: 100. No entry for role means no role restriction for that tab. Enter role on a single row per tab</t>
+  </si>
+  <si>
+    <t>caseworker-autotest2-solicitor</t>
   </si>
 </sst>
 </file>
@@ -891,7 +903,7 @@
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1095,6 +1107,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1210,7 +1228,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1317,6 +1335,10 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="4" applyAlignment="1"/>
     <xf numFmtId="49" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -2229,10 +2251,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2245,9 +2267,10 @@
     <col min="7" max="7" width="16.33203125" customWidth="1"/>
     <col min="8" max="8" width="40.83203125" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -2266,7 +2289,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
       <c r="C2" s="31" t="s">
@@ -2290,8 +2313,11 @@
       <c r="I2" s="30" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J2" s="76" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -2319,8 +2345,11 @@
       <c r="I3" s="8" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J3" s="77" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25">
         <v>42736</v>
       </c>
@@ -2347,7 +2376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27">
         <v>42736</v>
       </c>
@@ -2374,7 +2403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27">
         <v>42736</v>
       </c>
@@ -2401,7 +2430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27">
         <v>42736</v>
       </c>
@@ -2428,7 +2457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27">
         <v>42736</v>
       </c>
@@ -2455,7 +2484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27">
         <v>42736</v>
       </c>
@@ -2482,7 +2511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27">
         <v>42736</v>
       </c>
@@ -2509,7 +2538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27">
         <v>42736</v>
       </c>
@@ -2536,7 +2565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27">
         <v>42736</v>
       </c>
@@ -2563,7 +2592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27">
         <v>42736</v>
       </c>
@@ -2590,7 +2619,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="27">
         <v>42736</v>
       </c>
@@ -2617,7 +2646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="27">
         <v>42736</v>
       </c>
@@ -2644,7 +2673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27">
         <v>42736</v>
       </c>
@@ -2671,7 +2700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27">
         <v>42736</v>
       </c>
@@ -2698,7 +2727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="27">
         <v>42736</v>
       </c>
@@ -2725,7 +2754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="27">
         <v>42736</v>
       </c>
@@ -2752,7 +2781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="27">
         <v>42736</v>
       </c>
@@ -2764,130 +2793,133 @@
         <v>56</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>273</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>274</v>
+        <v>275</v>
+      </c>
+      <c r="F20" s="42" t="s">
+        <v>276</v>
       </c>
       <c r="G20" s="28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H20" s="42" t="s">
-        <v>269</v>
+        <v>225</v>
       </c>
       <c r="I20" s="28">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J20" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="27">
         <v>42736</v>
       </c>
       <c r="B21" s="27"/>
       <c r="C21" s="14" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="D21" s="28" t="s">
         <v>56</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>211</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>212</v>
+        <v>275</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>276</v>
       </c>
       <c r="G21" s="28">
-        <v>1</v>
-      </c>
-      <c r="H21" s="28" t="s">
-        <v>135</v>
+        <v>3</v>
+      </c>
+      <c r="H21" s="42" t="s">
+        <v>240</v>
       </c>
       <c r="I21" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="27">
         <v>42736</v>
       </c>
       <c r="B22" s="27"/>
       <c r="C22" s="14" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="D22" s="28" t="s">
         <v>56</v>
       </c>
       <c r="E22" s="42" t="s">
-        <v>211</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>212</v>
+        <v>275</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>276</v>
       </c>
       <c r="G22" s="28">
-        <v>1</v>
-      </c>
-      <c r="H22" s="28" t="s">
-        <v>137</v>
+        <v>3</v>
+      </c>
+      <c r="H22" s="42" t="s">
+        <v>243</v>
       </c>
       <c r="I22" s="28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="27">
         <v>42736</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="14" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="D23" s="28" t="s">
         <v>56</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>211</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>212</v>
+        <v>275</v>
+      </c>
+      <c r="F23" s="42" t="s">
+        <v>276</v>
       </c>
       <c r="G23" s="28">
-        <v>1</v>
-      </c>
-      <c r="H23" s="28" t="s">
-        <v>139</v>
+        <v>3</v>
+      </c>
+      <c r="H23" s="42" t="s">
+        <v>254</v>
       </c>
       <c r="I23" s="28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27">
         <v>42736</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="14" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="D24" s="28" t="s">
         <v>56</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>211</v>
+        <v>273</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>212</v>
+        <v>274</v>
       </c>
       <c r="G24" s="28">
+        <v>4</v>
+      </c>
+      <c r="H24" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="I24" s="28">
         <v>1</v>
       </c>
-      <c r="H24" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="I24" s="28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="27">
         <v>42736</v>
       </c>
@@ -2907,14 +2939,14 @@
       <c r="G25" s="28">
         <v>1</v>
       </c>
-      <c r="H25" s="42" t="s">
-        <v>146</v>
+      <c r="H25" s="28" t="s">
+        <v>135</v>
       </c>
       <c r="I25" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27">
         <v>42736</v>
       </c>
@@ -2926,22 +2958,22 @@
         <v>56</v>
       </c>
       <c r="E26" s="42" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G26" s="28">
+        <v>1</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="I26" s="28">
         <v>2</v>
       </c>
-      <c r="H26" s="42" t="s">
-        <v>150</v>
-      </c>
-      <c r="I26" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="27">
         <v>42736</v>
       </c>
@@ -2953,22 +2985,22 @@
         <v>56</v>
       </c>
       <c r="E27" s="42" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G27" s="28">
-        <v>2</v>
-      </c>
-      <c r="H27" s="42" t="s">
-        <v>158</v>
+        <v>1</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="I27" s="28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="27">
         <v>42736</v>
       </c>
@@ -2980,22 +3012,22 @@
         <v>56</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G28" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H28" s="42" t="s">
-        <v>247</v>
+        <v>144</v>
       </c>
       <c r="I28" s="28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="27">
         <v>42736</v>
       </c>
@@ -3007,22 +3039,22 @@
         <v>56</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G29" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H29" s="42" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="I29" s="28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="27">
         <v>42736</v>
       </c>
@@ -3043,13 +3075,13 @@
         <v>2</v>
       </c>
       <c r="H30" s="42" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="I30" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="27">
         <v>42736</v>
       </c>
@@ -3070,13 +3102,13 @@
         <v>2</v>
       </c>
       <c r="H31" s="42" t="s">
-        <v>258</v>
+        <v>158</v>
       </c>
       <c r="I31" s="28">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="27">
         <v>42736</v>
       </c>
@@ -3097,10 +3129,10 @@
         <v>2</v>
       </c>
       <c r="H32" s="42" t="s">
-        <v>170</v>
+        <v>247</v>
       </c>
       <c r="I32" s="28">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3115,19 +3147,19 @@
         <v>56</v>
       </c>
       <c r="E33" s="42" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="G33" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H33" s="42" t="s">
-        <v>225</v>
+        <v>156</v>
       </c>
       <c r="I33" s="28">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3142,19 +3174,19 @@
         <v>56</v>
       </c>
       <c r="E34" s="42" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="G34" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H34" s="42" t="s">
-        <v>240</v>
+        <v>160</v>
       </c>
       <c r="I34" s="28">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3169,19 +3201,19 @@
         <v>56</v>
       </c>
       <c r="E35" s="42" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="G35" s="28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H35" s="42" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="I35" s="28">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3196,30 +3228,138 @@
         <v>56</v>
       </c>
       <c r="E36" s="42" t="s">
+        <v>213</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="G36" s="28">
+        <v>2</v>
+      </c>
+      <c r="H36" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="I36" s="28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="27">
+        <v>42736</v>
+      </c>
+      <c r="B37" s="27"/>
+      <c r="C37" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="F37" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="G37" s="28">
+        <v>3</v>
+      </c>
+      <c r="H37" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="I37" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="27">
+        <v>42736</v>
+      </c>
+      <c r="B38" s="27"/>
+      <c r="C38" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="G38" s="28">
+        <v>3</v>
+      </c>
+      <c r="H38" s="42" t="s">
+        <v>240</v>
+      </c>
+      <c r="I38" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="27">
+        <v>42736</v>
+      </c>
+      <c r="B39" s="27"/>
+      <c r="C39" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="F39" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="G39" s="28">
+        <v>3</v>
+      </c>
+      <c r="H39" s="42" t="s">
+        <v>243</v>
+      </c>
+      <c r="I39" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="27">
+        <v>42736</v>
+      </c>
+      <c r="B40" s="27"/>
+      <c r="C40" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" s="42" t="s">
         <v>273</v>
       </c>
-      <c r="F36" s="21" t="s">
+      <c r="F40" s="21" t="s">
         <v>274</v>
       </c>
-      <c r="G36" s="28">
+      <c r="G40" s="28">
         <v>4</v>
       </c>
-      <c r="H36" s="42" t="s">
+      <c r="H40" s="42" t="s">
         <v>269</v>
       </c>
-      <c r="I36" s="28">
+      <c r="I40" s="28">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G36 I4:I36" xr:uid="{00000000-0002-0000-0C00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="I4:I40 G4:G40" xr:uid="{00000000-0002-0000-0C00-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A36" xr:uid="{00000000-0002-0000-0C00-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A40" xr:uid="{00000000-0002-0000-0C00-000002000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B36" xr:uid="{00000000-0002-0000-0C00-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B40" xr:uid="{00000000-0002-0000-0C00-000000000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -3897,8 +4037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
RDM-4362 revert excel file
</commit_message>
<xml_diff>
--- a/aat/src/resource/CCD_CNP_27.xlsx
+++ b/aat/src/resource/CCD_CNP_27.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/space/workspace/ccd-definition-store-api/aat/src/resource/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/code/ccd/ccd-definition-store-api/aat/src/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA53374-0933-8745-87CA-44EC347A41DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994F7540-D464-3047-B730-B47B7DA7E545}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1620" windowWidth="28800" windowHeight="15940" tabRatio="823" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1080" windowWidth="28800" windowHeight="15940" tabRatio="823" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1878" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1855" uniqueCount="275">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -880,18 +880,6 @@
   </si>
   <si>
     <t>History Tab</t>
-  </si>
-  <si>
-    <t>FourthTab</t>
-  </si>
-  <si>
-    <t>Fourth Tab</t>
-  </si>
-  <si>
-    <t>MaxLength: 100. No entry for role means no role restriction for that tab. Enter role on a single row per tab</t>
-  </si>
-  <si>
-    <t>caseworker-autotest2-solicitor</t>
   </si>
 </sst>
 </file>
@@ -903,7 +891,7 @@
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1107,12 +1095,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1228,7 +1210,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1335,10 +1317,6 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="4" applyAlignment="1"/>
     <xf numFmtId="49" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -2251,10 +2229,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2267,10 +2245,9 @@
     <col min="7" max="7" width="16.33203125" customWidth="1"/>
     <col min="8" max="8" width="40.83203125" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -2289,7 +2266,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:10" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
       <c r="C2" s="31" t="s">
@@ -2313,11 +2290,8 @@
       <c r="I2" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="76" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -2345,11 +2319,8 @@
       <c r="I3" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="J3" s="77" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25">
         <v>42736</v>
       </c>
@@ -2376,7 +2347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27">
         <v>42736</v>
       </c>
@@ -2403,7 +2374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27">
         <v>42736</v>
       </c>
@@ -2430,7 +2401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27">
         <v>42736</v>
       </c>
@@ -2457,7 +2428,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27">
         <v>42736</v>
       </c>
@@ -2484,7 +2455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27">
         <v>42736</v>
       </c>
@@ -2511,7 +2482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27">
         <v>42736</v>
       </c>
@@ -2538,7 +2509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27">
         <v>42736</v>
       </c>
@@ -2565,7 +2536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27">
         <v>42736</v>
       </c>
@@ -2592,7 +2563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27">
         <v>42736</v>
       </c>
@@ -2619,7 +2590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="27">
         <v>42736</v>
       </c>
@@ -2646,7 +2617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="27">
         <v>42736</v>
       </c>
@@ -2673,7 +2644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27">
         <v>42736</v>
       </c>
@@ -2700,7 +2671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27">
         <v>42736</v>
       </c>
@@ -2727,7 +2698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="27">
         <v>42736</v>
       </c>
@@ -2754,7 +2725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="27">
         <v>42736</v>
       </c>
@@ -2781,7 +2752,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="27">
         <v>42736</v>
       </c>
@@ -2793,133 +2764,130 @@
         <v>56</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>275</v>
-      </c>
-      <c r="F20" s="42" t="s">
-        <v>276</v>
+        <v>273</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>274</v>
       </c>
       <c r="G20" s="28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H20" s="42" t="s">
-        <v>225</v>
+        <v>269</v>
       </c>
       <c r="I20" s="28">
         <v>1</v>
       </c>
-      <c r="J20" s="14" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="21" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="27">
         <v>42736</v>
       </c>
       <c r="B21" s="27"/>
       <c r="C21" s="14" t="s">
-        <v>234</v>
+        <v>251</v>
       </c>
       <c r="D21" s="28" t="s">
         <v>56</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>275</v>
-      </c>
-      <c r="F21" s="42" t="s">
-        <v>276</v>
+        <v>211</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>212</v>
       </c>
       <c r="G21" s="28">
-        <v>3</v>
-      </c>
-      <c r="H21" s="42" t="s">
-        <v>240</v>
+        <v>1</v>
+      </c>
+      <c r="H21" s="28" t="s">
+        <v>135</v>
       </c>
       <c r="I21" s="28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="27">
         <v>42736</v>
       </c>
       <c r="B22" s="27"/>
       <c r="C22" s="14" t="s">
-        <v>234</v>
+        <v>251</v>
       </c>
       <c r="D22" s="28" t="s">
         <v>56</v>
       </c>
       <c r="E22" s="42" t="s">
-        <v>275</v>
-      </c>
-      <c r="F22" s="42" t="s">
-        <v>276</v>
+        <v>211</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>212</v>
       </c>
       <c r="G22" s="28">
-        <v>3</v>
-      </c>
-      <c r="H22" s="42" t="s">
-        <v>243</v>
+        <v>1</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>137</v>
       </c>
       <c r="I22" s="28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="27">
         <v>42736</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="14" t="s">
-        <v>234</v>
+        <v>251</v>
       </c>
       <c r="D23" s="28" t="s">
         <v>56</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>275</v>
-      </c>
-      <c r="F23" s="42" t="s">
-        <v>276</v>
+        <v>211</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>212</v>
       </c>
       <c r="G23" s="28">
+        <v>1</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="I23" s="28">
         <v>3</v>
       </c>
-      <c r="H23" s="42" t="s">
-        <v>254</v>
-      </c>
-      <c r="I23" s="28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27">
         <v>42736</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="14" t="s">
-        <v>234</v>
+        <v>251</v>
       </c>
       <c r="D24" s="28" t="s">
         <v>56</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>273</v>
+        <v>211</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>274</v>
+        <v>212</v>
       </c>
       <c r="G24" s="28">
+        <v>1</v>
+      </c>
+      <c r="H24" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="I24" s="28">
         <v>4</v>
       </c>
-      <c r="H24" s="42" t="s">
-        <v>269</v>
-      </c>
-      <c r="I24" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="27">
         <v>42736</v>
       </c>
@@ -2939,14 +2907,14 @@
       <c r="G25" s="28">
         <v>1</v>
       </c>
-      <c r="H25" s="28" t="s">
-        <v>135</v>
+      <c r="H25" s="42" t="s">
+        <v>146</v>
       </c>
       <c r="I25" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27">
         <v>42736</v>
       </c>
@@ -2958,22 +2926,22 @@
         <v>56</v>
       </c>
       <c r="E26" s="42" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G26" s="28">
+        <v>2</v>
+      </c>
+      <c r="H26" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="I26" s="28">
         <v>1</v>
       </c>
-      <c r="H26" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="I26" s="28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="27">
         <v>42736</v>
       </c>
@@ -2985,22 +2953,22 @@
         <v>56</v>
       </c>
       <c r="E27" s="42" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G27" s="28">
-        <v>1</v>
-      </c>
-      <c r="H27" s="28" t="s">
-        <v>139</v>
+        <v>2</v>
+      </c>
+      <c r="H27" s="42" t="s">
+        <v>158</v>
       </c>
       <c r="I27" s="28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="27">
         <v>42736</v>
       </c>
@@ -3012,22 +2980,22 @@
         <v>56</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G28" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28" s="42" t="s">
-        <v>144</v>
+        <v>247</v>
       </c>
       <c r="I28" s="28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="27">
         <v>42736</v>
       </c>
@@ -3039,22 +3007,22 @@
         <v>56</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G29" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H29" s="42" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="I29" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="27">
         <v>42736</v>
       </c>
@@ -3075,13 +3043,13 @@
         <v>2</v>
       </c>
       <c r="H30" s="42" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="I30" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="27">
         <v>42736</v>
       </c>
@@ -3102,13 +3070,13 @@
         <v>2</v>
       </c>
       <c r="H31" s="42" t="s">
-        <v>158</v>
+        <v>258</v>
       </c>
       <c r="I31" s="28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="27">
         <v>42736</v>
       </c>
@@ -3129,10 +3097,10 @@
         <v>2</v>
       </c>
       <c r="H32" s="42" t="s">
-        <v>247</v>
+        <v>170</v>
       </c>
       <c r="I32" s="28">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3147,19 +3115,19 @@
         <v>56</v>
       </c>
       <c r="E33" s="42" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="G33" s="28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H33" s="42" t="s">
-        <v>156</v>
+        <v>225</v>
       </c>
       <c r="I33" s="28">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3174,19 +3142,19 @@
         <v>56</v>
       </c>
       <c r="E34" s="42" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="G34" s="28">
+        <v>3</v>
+      </c>
+      <c r="H34" s="42" t="s">
+        <v>240</v>
+      </c>
+      <c r="I34" s="28">
         <v>2</v>
-      </c>
-      <c r="H34" s="42" t="s">
-        <v>160</v>
-      </c>
-      <c r="I34" s="28">
-        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3201,19 +3169,19 @@
         <v>56</v>
       </c>
       <c r="E35" s="42" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="G35" s="28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H35" s="42" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="I35" s="28">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3228,138 +3196,30 @@
         <v>56</v>
       </c>
       <c r="E36" s="42" t="s">
-        <v>213</v>
+        <v>273</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>214</v>
+        <v>274</v>
       </c>
       <c r="G36" s="28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H36" s="42" t="s">
-        <v>170</v>
+        <v>269</v>
       </c>
       <c r="I36" s="28">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="27">
-        <v>42736</v>
-      </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E37" s="42" t="s">
-        <v>232</v>
-      </c>
-      <c r="F37" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="G37" s="28">
-        <v>3</v>
-      </c>
-      <c r="H37" s="42" t="s">
-        <v>225</v>
-      </c>
-      <c r="I37" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="27">
-        <v>42736</v>
-      </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="D38" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E38" s="42" t="s">
-        <v>232</v>
-      </c>
-      <c r="F38" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="G38" s="28">
-        <v>3</v>
-      </c>
-      <c r="H38" s="42" t="s">
-        <v>240</v>
-      </c>
-      <c r="I38" s="28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="27">
-        <v>42736</v>
-      </c>
-      <c r="B39" s="27"/>
-      <c r="C39" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="D39" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E39" s="42" t="s">
-        <v>232</v>
-      </c>
-      <c r="F39" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="G39" s="28">
-        <v>3</v>
-      </c>
-      <c r="H39" s="42" t="s">
-        <v>243</v>
-      </c>
-      <c r="I39" s="28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="27">
-        <v>42736</v>
-      </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="D40" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E40" s="42" t="s">
-        <v>273</v>
-      </c>
-      <c r="F40" s="21" t="s">
-        <v>274</v>
-      </c>
-      <c r="G40" s="28">
-        <v>4</v>
-      </c>
-      <c r="H40" s="42" t="s">
-        <v>269</v>
-      </c>
-      <c r="I40" s="28">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="I4:I40 G4:G40" xr:uid="{00000000-0002-0000-0C00-000001000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number greater than 0" sqref="G4:G36 I4:I36" xr:uid="{00000000-0002-0000-0C00-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A40" xr:uid="{00000000-0002-0000-0C00-000002000000}">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A36" xr:uid="{00000000-0002-0000-0C00-000002000000}">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B40" xr:uid="{00000000-0002-0000-0C00-000000000000}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date after 'LiveFrom' date" sqref="B4:B36" xr:uid="{00000000-0002-0000-0C00-000000000000}">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -4037,8 +3897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
RDM-4084 Update tests fix validation of complex parents add complex ACLs to the API
</commit_message>
<xml_diff>
--- a/aat/src/resource/CCD_CNP_27.xlsx
+++ b/aat/src/resource/CCD_CNP_27.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev/code/ccd/ccd-definition-store-api/aat/src/resource/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/space/workspace/ccd-definition-store-api/aat/src/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994F7540-D464-3047-B730-B47B7DA7E545}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBA4FFD-D72A-6A45-BD49-BE7682F107D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="28800" windowHeight="15940" tabRatio="823" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1080" windowWidth="28800" windowHeight="15940" tabRatio="823" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId16"/>
     <sheet name="AuthorisationCaseEvent" sheetId="15" r:id="rId17"/>
     <sheet name="AuthorisationCaseField" sheetId="14" r:id="rId18"/>
+    <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="140001"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1855" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1871" uniqueCount="281">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -880,6 +881,29 @@
   </si>
   <si>
     <t>History Tab</t>
+  </si>
+  <si>
+    <t>AuthorisationComplexType</t>
+  </si>
+  <si>
+    <t>Must match ID on 'CaseType' tab
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>The Field ID should match an ID in the CaseField Tab
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>The complex type element (field) ID (ListElementId) should match the field attribute name used by the service team in creating the case
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Must match ID role.  If a role doesn’t have a Row below that mean no access to.
+MaxLength: 100.</t>
+  </si>
+  <si>
+    <t>C - Create, R - Read, U - Update, D - Delete
+MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
   </si>
 </sst>
 </file>
@@ -891,7 +915,7 @@
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1095,6 +1119,81 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF984807"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1182,7 +1281,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1209,8 +1308,11 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1317,8 +1419,23 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="4" applyAlignment="1"/>
     <xf numFmtId="49" fontId="9" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="26" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="26" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="26" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="26" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="26"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="27"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="26" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="26" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="26" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="26" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="26" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="26">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1345,6 +1462,9 @@
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Normal 2 3" xfId="26" xr:uid="{B75572D7-6A12-2E4F-BFA2-198FB3AC3812}"/>
+    <cellStyle name="Normal 3" xfId="27" xr:uid="{63780BEC-AE4D-934E-9473-A01E2AF084BD}"/>
+    <cellStyle name="Normal 3 2" xfId="28" xr:uid="{1FA08255-7C4C-8944-85A6-8E22F65BB926}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3897,7 +4017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -4532,6 +4652,90 @@
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" style="81" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="81" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="81" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="81" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.6640625" style="81" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="81" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="81" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="81"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="76" t="s">
+        <v>275</v>
+      </c>
+      <c r="B1" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="78" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="79" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+    </row>
+    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
+      <c r="A2" s="82"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="83" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" s="83" t="s">
+        <v>277</v>
+      </c>
+      <c r="E2" s="83" t="s">
+        <v>278</v>
+      </c>
+      <c r="F2" s="83" t="s">
+        <v>279</v>
+      </c>
+      <c r="G2" s="83" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="84" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="85" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="86" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="86" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
RDM-4084 add configuration data for complex type authorisation and relevant functional tests
</commit_message>
<xml_diff>
--- a/aat/src/resource/CCD_CNP_27.xlsx
+++ b/aat/src/resource/CCD_CNP_27.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/space/workspace/ccd-definition-store-api/aat/src/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBA4FFD-D72A-6A45-BD49-BE7682F107D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303EB6FC-0E41-F14C-A42F-4396C6198147}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="28800" windowHeight="15940" tabRatio="823" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1080" windowWidth="29180" windowHeight="16620" tabRatio="823" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1871" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1886" uniqueCount="281">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -4017,8 +4017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4657,10 +4657,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4732,6 +4732,66 @@
       </c>
       <c r="G3" s="86" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="72">
+        <v>42736</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="G4" s="81" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="72">
+        <v>42736</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>217</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="G5" s="81" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="72">
+        <v>42736</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>223</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="G6" s="81" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4899,7 +4959,7 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6252,7 +6312,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D6" sqref="D6:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>